<commit_message>
Excel is working now. Updated chrome driver
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/datasheets/TestData.xlsx
+++ b/Demo/src/test/resources/datasheets/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aadit\git\SeleniumDemo\Demo\src\test\resources\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45611AC3-6043-4035-AE72-7EABE0F83BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209314E9-6884-4179-B7A6-4E856E7E473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4776" yWindow="3384" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>TC001_sampleTest</t>
   </si>
   <si>
-    <t>mngr299483</t>
-  </si>
-  <si>
-    <t>suqUpej</t>
+    <t>mngr332130</t>
+  </si>
+  <si>
+    <t>EdAbAda</t>
   </si>
 </sst>
 </file>
@@ -363,15 +363,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>